<commit_message>
CHUC nang sua tai khoan
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="7812" windowHeight="5484" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DangNhap" sheetId="1" r:id="rId1"/>
     <sheet name="DangKi" sheetId="2" r:id="rId2"/>
     <sheet name="MuaHang" sheetId="3" r:id="rId3"/>
+    <sheet name="SuaTaiKhoan" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:D17"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -101,13 +101,31 @@
   </si>
   <si>
     <t>Đặt hàng thành công!</t>
+  </si>
+  <si>
+    <t>sodienthoai</t>
+  </si>
+  <si>
+    <t>MatKhau</t>
+  </si>
+  <si>
+    <t>Tô Thị Duyên</t>
+  </si>
+  <si>
+    <t>`0343654251</t>
+  </si>
+  <si>
+    <t>Thay đổi thông tin thành công!</t>
+  </si>
+  <si>
+    <t>matkhaumoi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +138,26 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,17 +177,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -557,10 +599,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,6 +748,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>123456</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -713,10 +772,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,12 +897,29 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -851,4 +927,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>